<commit_message>
P3 IMC Parte 10
</commit_message>
<xml_diff>
--- a/IntroducionModelosComputacionales/Practica3/Tablas Excel.xlsx
+++ b/IntroducionModelosComputacionales/Practica3/Tablas Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITHUB\Practicas4Computacion\IntroducionModelosComputacionales\Practica3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54273280-9132-4E33-B311-1E61ECD9C4E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BE3CF5-2117-4088-BBC1-E4CC97E31B64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12528" yWindow="1164" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12765" yWindow="1185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -275,12 +275,6 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -375,6 +369,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -435,12 +435,6 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -535,6 +529,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -595,12 +595,6 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -695,6 +689,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -755,12 +755,6 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -855,6 +849,12 @@
     <dxf>
       <font>
         <b/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -915,12 +915,6 @@
     <dxf>
       <font>
         <b/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1009,6 +1003,12 @@
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1095,11 +1095,11 @@
     <filterColumn colId="4" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="56" totalsRowDxfId="57"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="5%" dataDxfId="54" totalsRowDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="15%" dataDxfId="52" totalsRowDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25%" dataDxfId="50" totalsRowDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="50%" totalsRowFunction="count" dataDxfId="48" totalsRowDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="5%" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="15%" dataDxfId="53" totalsRowDxfId="52"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="25%" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="50%" totalsRowFunction="count" dataDxfId="49" totalsRowDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1109,11 +1109,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{932A1EFA-F95A-4043-9727-67D57E33952A}" name="Tabla35" displayName="Tabla35" ref="C24:G28" headerRowDxfId="47" dataDxfId="46">
   <autoFilter ref="C24:G28" xr:uid="{7E7A20F1-1FE1-4C00-94CF-040C128FAA07}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0CF1D07E-F69F-41B3-B1A6-5271D0328327}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="44" totalsRowDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{D6EE76ED-501A-4B9C-9682-E09B946C0B1F}" name="5%" dataDxfId="42" totalsRowDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{FD77CE01-BF37-4247-A4E3-D2B3DC81119A}" name="15%" dataDxfId="40" totalsRowDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{F510BE8F-4436-4F75-8C37-63C9F374D818}" name="25%" dataDxfId="38" totalsRowDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{284E5899-0EEF-49CE-A816-EC8F01DDFE26}" name="50%" totalsRowFunction="count" dataDxfId="36" totalsRowDxfId="37"/>
+    <tableColumn id="1" xr3:uid="{0CF1D07E-F69F-41B3-B1A6-5271D0328327}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{D6EE76ED-501A-4B9C-9682-E09B946C0B1F}" name="5%" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{FD77CE01-BF37-4247-A4E3-D2B3DC81119A}" name="15%" dataDxfId="41" totalsRowDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{F510BE8F-4436-4F75-8C37-63C9F374D818}" name="25%" dataDxfId="39" totalsRowDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{284E5899-0EEF-49CE-A816-EC8F01DDFE26}" name="50%" totalsRowFunction="count" dataDxfId="37" totalsRowDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1123,11 +1123,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{213FDFFA-70E3-44D3-8AFF-9C6EB3A154D8}" name="Tabla357" displayName="Tabla357" ref="C44:G48" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="C44:G48" xr:uid="{19A516D0-5219-4680-80FE-925E81815CC4}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{EC4511A6-AB21-473C-93AA-A330F237EE19}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="32" totalsRowDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{51986169-24F4-4D82-90AA-6F22E8BE3DA8}" name="5%" dataDxfId="30" totalsRowDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{29B39A0D-F5A6-49EF-9D59-42D81A77C8D0}" name="15%" dataDxfId="28" totalsRowDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{8A71A8FA-EB2B-4405-AFA4-95430B63A727}" name="25%" dataDxfId="26" totalsRowDxfId="27"/>
-    <tableColumn id="5" xr3:uid="{72C4101B-F63F-484D-9BA3-65EC5E6E540D}" name="50%" totalsRowFunction="count" dataDxfId="24" totalsRowDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{EC4511A6-AB21-473C-93AA-A330F237EE19}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{51986169-24F4-4D82-90AA-6F22E8BE3DA8}" name="5%" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{29B39A0D-F5A6-49EF-9D59-42D81A77C8D0}" name="15%" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{8A71A8FA-EB2B-4405-AFA4-95430B63A727}" name="25%" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{72C4101B-F63F-484D-9BA3-65EC5E6E540D}" name="50%" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1137,11 +1137,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1C647B78-C84E-4C14-B3BD-38069C98429F}" name="Tabla3578" displayName="Tabla3578" ref="C66:G70" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="C66:G70" xr:uid="{278B819D-5199-40FC-82B2-840A2759536D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{A6985645-76DA-43AB-B5F5-40AB32AB81A8}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{F1470ACD-178B-4F03-8407-277C1537CAEE}" name="5%" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{56A3261E-6EF9-430A-8CFF-ED3D59D95D15}" name="15%" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{BF14D909-C533-4C20-A69D-946CED6D6D0F}" name="25%" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{2E953B70-8C41-487F-B1E3-C0064AAF5BD3}" name="50%" totalsRowFunction="count" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{A6985645-76DA-43AB-B5F5-40AB32AB81A8}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{F1470ACD-178B-4F03-8407-277C1537CAEE}" name="5%" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{56A3261E-6EF9-430A-8CFF-ED3D59D95D15}" name="15%" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{BF14D909-C533-4C20-A69D-946CED6D6D0F}" name="25%" dataDxfId="15" totalsRowDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{2E953B70-8C41-487F-B1E3-C0064AAF5BD3}" name="50%" totalsRowFunction="count" dataDxfId="13" totalsRowDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1151,11 +1151,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{6281AC80-40E5-424F-9291-B7FDE85F1783}" name="Tabla357810" displayName="Tabla357810" ref="C92:G96" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="C92:G96" xr:uid="{C613B308-06DF-4BB7-9F69-03A7A902EB85}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0B63ECC6-6F54-437A-AD00-10FAF662583B}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{75324B59-08AB-4D90-8D48-553C01D2761C}" name="5%" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{05C11C1D-F8BF-4AAF-A2D4-936AEB32241D}" name="15%" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{43D7D313-0EE3-4D66-8C86-9CB6BFF2615C}" name="25%" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{DDC79F7E-72B5-4E6C-9B82-0BB951916D4A}" name="50%" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{0B63ECC6-6F54-437A-AD00-10FAF662583B}" name="PORCENTAJE DE NODOS" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{75324B59-08AB-4D90-8D48-553C01D2761C}" name="5%" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{05C11C1D-F8BF-4AAF-A2D4-936AEB32241D}" name="15%" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{43D7D313-0EE3-4D66-8C86-9CB6BFF2615C}" name="25%" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{DDC79F7E-72B5-4E6C-9B82-0BB951916D4A}" name="50%" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1460,34 +1460,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:P135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C88" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="49.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="31.88671875" customWidth="1"/>
-    <col min="4" max="4" width="22.5546875" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F3" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>0.11472</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>0.195356</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1546,36 +1546,36 @@
         <v>7</v>
       </c>
       <c r="D8" s="5">
-        <v>0</v>
+        <v>80.33</v>
       </c>
       <c r="E8" s="5">
-        <v>0</v>
+        <v>78.33</v>
       </c>
       <c r="F8" s="5">
-        <v>0</v>
+        <v>79.5</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+        <v>80.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="5">
-        <v>0</v>
+        <v>78.05</v>
       </c>
       <c r="E9" s="5">
-        <v>0</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="F9" s="5">
-        <v>0</v>
+        <v>67.8</v>
       </c>
       <c r="G9" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+        <v>69.27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
         <v>12</v>
       </c>
@@ -1592,7 +1592,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1.1580999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>5</v>
       </c>
@@ -1629,52 +1629,52 @@
         <v>0.18731600000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="6">
-        <v>0</v>
+        <v>79.67</v>
       </c>
       <c r="E17" s="6">
-        <v>0</v>
+        <v>78.5</v>
       </c>
       <c r="F17" s="6">
-        <v>0</v>
+        <v>78.33</v>
       </c>
       <c r="G17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>80.67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D18" s="6">
-        <v>0</v>
+        <v>78.05</v>
       </c>
       <c r="E18" s="6">
-        <v>0</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="F18" s="6">
-        <v>0</v>
+        <v>65.849999999999994</v>
       </c>
       <c r="G18" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+        <v>68.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
     </row>
-    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F22" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>2.6151000000000001E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C26" s="1" t="s">
         <v>5</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>3.5325000000000002E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>13</v>
       </c>
@@ -1733,36 +1733,36 @@
         <v>7</v>
       </c>
       <c r="D27" s="5">
-        <v>0</v>
+        <v>94.54</v>
       </c>
       <c r="E27" s="5">
-        <v>0</v>
+        <v>94.73</v>
       </c>
       <c r="F27" s="5">
-        <v>0</v>
+        <v>94.73</v>
       </c>
       <c r="G27" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+        <v>94.73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D28" s="5">
-        <v>0</v>
+        <v>94.87</v>
       </c>
       <c r="E28" s="5">
-        <v>0</v>
+        <v>94.39</v>
       </c>
       <c r="F28" s="5">
-        <v>0</v>
+        <v>93.8</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+        <v>93.91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C33" s="10" t="s">
         <v>12</v>
       </c>
@@ -1779,7 +1779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>2.6120000000000001E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C35" s="3" t="s">
         <v>5</v>
       </c>
@@ -1816,46 +1816,46 @@
         <v>3.0800000000000001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="6">
-        <v>0</v>
+        <v>94.57</v>
       </c>
       <c r="E36" s="6">
-        <v>0</v>
+        <v>94.72</v>
       </c>
       <c r="F36" s="6">
-        <v>0</v>
+        <v>94.73</v>
       </c>
       <c r="G36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+        <v>94.73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D37" s="6">
-        <v>0</v>
+        <v>94.83</v>
       </c>
       <c r="E37" s="6">
-        <v>0</v>
+        <v>94.25</v>
       </c>
       <c r="F37" s="6">
-        <v>0</v>
+        <v>94.28</v>
       </c>
       <c r="G37" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>94.13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F42" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C44" s="1" t="s">
         <v>12</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C45" s="1" t="s">
         <v>4</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>1.34E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="s">
         <v>5</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>1.155E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>13</v>
       </c>
@@ -1914,36 +1914,36 @@
         <v>7</v>
       </c>
       <c r="D47" s="5">
-        <v>0</v>
+        <v>96.37</v>
       </c>
       <c r="E47" s="5">
-        <v>0</v>
+        <v>97.5</v>
       </c>
       <c r="F47" s="5">
-        <v>0</v>
+        <v>98.26</v>
       </c>
       <c r="G47" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+        <v>98.99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C48" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D48" s="5">
-        <v>0</v>
+        <v>96.54</v>
       </c>
       <c r="E48" s="5">
-        <v>0</v>
+        <v>97.06</v>
       </c>
       <c r="F48" s="5">
-        <v>0</v>
+        <v>97.36</v>
       </c>
       <c r="G48" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+        <v>97.51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C53" s="10" t="s">
         <v>12</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>14</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>1.44E-4</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C55" s="3" t="s">
         <v>5</v>
       </c>
@@ -1997,46 +1997,46 @@
         <v>1.807E-3</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="6">
-        <v>0</v>
+        <v>96.45</v>
       </c>
       <c r="E56" s="6">
-        <v>0</v>
+        <v>97.74</v>
       </c>
       <c r="F56" s="6">
-        <v>0</v>
+        <v>98.21</v>
       </c>
       <c r="G56" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99.06</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C57" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D57" s="6">
-        <v>0</v>
+        <v>96.85</v>
       </c>
       <c r="E57" s="6">
-        <v>0</v>
+        <v>97.14</v>
       </c>
       <c r="F57" s="6">
-        <v>0</v>
+        <v>97.33</v>
       </c>
       <c r="G57" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+        <v>96.86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F64" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>12</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>4</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>6.1349999999999998E-3</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C68" s="1" t="s">
         <v>5</v>
       </c>
@@ -2087,7 +2087,7 @@
         <v>6.2385000000000003E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>17</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>99.39</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>6</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>93.76</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C74" s="10" t="s">
         <v>18</v>
       </c>
@@ -2147,7 +2147,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C75" s="10" t="s">
         <v>19</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>21</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>6.1349999999999998E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C77" s="3" t="s">
         <v>5</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>3.6700000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C78" s="3" t="s">
         <v>7</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>99.39</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C79" s="3" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>93.76</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C81" s="10" t="s">
         <v>18</v>
       </c>
@@ -2288,7 +2288,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C82" s="10" t="s">
         <v>19</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>23</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>6.1349999999999998E-3</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C84" s="3" t="s">
         <v>5</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>6.4219999999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C85" s="3" t="s">
         <v>7</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>99.39</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C86" s="3" t="s">
         <v>6</v>
       </c>
@@ -2406,12 +2406,12 @@
         <v>93.58</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F90" s="7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C92" s="1" t="s">
         <v>12</v>
       </c>
@@ -2428,41 +2428,41 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C93" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D93" s="5">
-        <v>0.73844399999999999</v>
+        <v>3.6211E-2</v>
       </c>
       <c r="E93" s="5">
-        <v>0.53688899999999995</v>
+        <v>1</v>
       </c>
       <c r="F93" s="5">
-        <v>0.45133299999999998</v>
+        <v>3.3000000000000003E-5</v>
       </c>
       <c r="G93" s="5">
-        <v>0.21333299999999999</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.8E-5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C94" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D94" s="5">
-        <v>0.87733300000000003</v>
+        <v>3.3066999999999999E-2</v>
       </c>
       <c r="E94" s="5">
-        <v>0.69666700000000004</v>
+        <v>4.3270000000000003E-2</v>
       </c>
       <c r="F94" s="5">
-        <v>0.61866699999999997</v>
+        <v>3.9870000000000003E-2</v>
       </c>
       <c r="G94" s="5">
-        <v>0.61599999999999999</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+        <v>3.5126999999999999E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>17</v>
       </c>
@@ -2473,16 +2473,16 @@
         <v>88.11</v>
       </c>
       <c r="E95" s="5">
-        <v>91.33</v>
+        <v>100</v>
       </c>
       <c r="F95" s="5">
-        <v>93.2</v>
+        <v>100</v>
       </c>
       <c r="G95" s="5">
-        <v>96.16</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C96" s="1" t="s">
         <v>6</v>
       </c>
@@ -2490,16 +2490,16 @@
         <v>88.67</v>
       </c>
       <c r="E96" s="5">
-        <v>91.2</v>
+        <v>86.2</v>
       </c>
       <c r="F96" s="5">
-        <v>91.6</v>
+        <v>86.73</v>
       </c>
       <c r="G96" s="5">
-        <v>93.7</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C100" s="10" t="s">
         <v>18</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C101" s="10" t="s">
         <v>19</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>21</v>
       </c>
@@ -2553,48 +2553,48 @@
         <v>4</v>
       </c>
       <c r="D102" s="6">
-        <v>0.80444400000000005</v>
+        <v>4.2464000000000002E-2</v>
       </c>
       <c r="E102" s="6">
-        <v>0.15044299999999999</v>
+        <v>1.1048000000000001E-2</v>
       </c>
       <c r="F102" s="6">
-        <v>2.22E-4</v>
+        <v>8.8999999999999995E-4</v>
       </c>
       <c r="G102" s="9">
-        <v>0</v>
+        <v>6.2000000000000003E-5</v>
       </c>
       <c r="H102" s="6">
-        <v>0</v>
+        <v>2.0999999999999999E-5</v>
       </c>
       <c r="I102" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.8E-5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C103" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D103" s="6">
-        <v>0.71199999999999997</v>
+        <v>3.9845600000000002E-2</v>
       </c>
       <c r="E103" s="6">
-        <v>0.64402139999999997</v>
+        <v>2.3820999999999998E-2</v>
       </c>
       <c r="F103" s="6">
-        <v>0.76800000000000002</v>
+        <v>3.0034999999999999E-2</v>
       </c>
       <c r="G103" s="9">
-        <v>0.80666669999999996</v>
+        <v>3.3804500000000001E-2</v>
       </c>
       <c r="H103" s="6">
-        <v>0.81730000000000003</v>
+        <v>0.35009000000000001</v>
       </c>
       <c r="I103" s="6">
-        <v>0.81266700000000003</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.5126999999999999E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C104" s="3" t="s">
         <v>7</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C105" s="3" t="s">
         <v>6</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C107" s="10" t="s">
         <v>18</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C108" s="10" t="s">
         <v>19</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>23</v>
       </c>
@@ -2694,48 +2694,48 @@
         <v>4</v>
       </c>
       <c r="D109" s="6">
-        <v>0.67</v>
+        <v>3.5389999999999998E-2</v>
       </c>
       <c r="E109" s="6">
-        <v>0.31466699999999997</v>
+        <v>1.818055E-2</v>
       </c>
       <c r="F109" s="6">
-        <v>6.0888999999999999E-2</v>
+        <v>6.3610000000000003E-3</v>
       </c>
       <c r="G109" s="9">
-        <v>0</v>
+        <v>8.4099999999999995E-4</v>
       </c>
       <c r="H109" s="6">
-        <v>0</v>
+        <v>4.3000000000000002E-5</v>
       </c>
       <c r="I109" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+        <v>1.9999999999999999E-6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C110" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D110" s="6">
-        <v>0.65400000000000003</v>
+        <v>3.4311000000000001E-2</v>
       </c>
       <c r="E110" s="6">
-        <v>0.65856400000000004</v>
+        <v>2.4514999999999999E-2</v>
       </c>
       <c r="F110" s="6">
-        <v>0.66266700000000001</v>
+        <v>2.4888E-2</v>
       </c>
       <c r="G110" s="9">
-        <v>0.80300000000000005</v>
+        <v>3.0487E-2</v>
       </c>
       <c r="H110" s="6">
-        <v>0.83</v>
+        <v>3.4533000000000001E-2</v>
       </c>
       <c r="I110" s="6">
-        <v>0.85333000000000003</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+        <v>3.6739000000000001E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C111" s="3" t="s">
         <v>7</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>94.67</v>
       </c>
       <c r="F111" s="6">
-        <v>98.76</v>
+        <v>98.79</v>
       </c>
       <c r="G111" s="9">
         <v>100</v>
@@ -2758,7 +2758,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C112" s="3" t="s">
         <v>6</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>90.87</v>
       </c>
       <c r="E112" s="6">
-        <v>91.63</v>
+        <v>91.6</v>
       </c>
       <c r="F112" s="6">
         <v>90.33</v>
@@ -2775,13 +2775,13 @@
         <v>88.33</v>
       </c>
       <c r="H112" s="6">
-        <v>0.88</v>
+        <v>88</v>
       </c>
       <c r="I112" s="6">
-        <v>87.73</v>
-      </c>
-    </row>
-    <row r="135" spans="10:10" x14ac:dyDescent="0.3">
+        <v>87.6</v>
+      </c>
+    </row>
+    <row r="135" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J135" t="s">
         <v>3</v>
       </c>
@@ -2789,7 +2789,7 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="H10">
-    <cfRule type="colorScale" priority="124">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2801,7 +2801,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:G7">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2813,7 +2813,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:G9">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2825,6 +2825,162 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6:G6">
+    <cfRule type="colorScale" priority="66">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16:G16">
+    <cfRule type="colorScale" priority="65">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:G18">
+    <cfRule type="colorScale" priority="64">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15:G15">
+    <cfRule type="colorScale" priority="63">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D26:G26">
+    <cfRule type="colorScale" priority="62">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:G28">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:G25">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:G35">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:G37">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D34:G34">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:G46">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:G48">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:G45">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D55:G55">
     <cfRule type="colorScale" priority="53">
       <colorScale>
         <cfvo type="min"/>
@@ -2836,7 +2992,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:G16">
+  <conditionalFormatting sqref="D56:G57">
     <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
@@ -2848,7 +3004,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17:G18">
+  <conditionalFormatting sqref="D54:G54">
     <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
@@ -2860,7 +3016,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:G15">
+  <conditionalFormatting sqref="D68:G68">
     <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
@@ -2872,19 +3028,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26:G26">
-    <cfRule type="colorScale" priority="49">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:G28">
+  <conditionalFormatting sqref="D69:G70">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D67:G67">
     <cfRule type="colorScale" priority="48">
       <colorScale>
         <cfvo type="min"/>
@@ -2896,7 +3052,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:G25">
+  <conditionalFormatting sqref="D77:G77">
     <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
@@ -2908,7 +3064,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35:G35">
+  <conditionalFormatting sqref="D78:G79">
     <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
@@ -2920,7 +3076,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36:G37">
+  <conditionalFormatting sqref="D76:G76">
     <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
@@ -2932,19 +3088,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34:G34">
-    <cfRule type="colorScale" priority="44">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D46:G46">
+  <conditionalFormatting sqref="H77:I77">
     <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="min"/>
@@ -2956,7 +3100,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47:G48">
+  <conditionalFormatting sqref="H78:I79">
     <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
@@ -2968,7 +3112,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45:G45">
+  <conditionalFormatting sqref="H76:I76">
     <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
@@ -2980,7 +3124,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D55:G55">
+  <conditionalFormatting sqref="D84:G84">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
@@ -2992,7 +3136,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:G57">
+  <conditionalFormatting sqref="D85:G86">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -3004,7 +3148,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D54:G54">
+  <conditionalFormatting sqref="D83:G83">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -3016,7 +3160,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D68:G68">
+  <conditionalFormatting sqref="H84:I84">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
@@ -3028,67 +3172,91 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D69:G70">
+  <conditionalFormatting sqref="H85:I86">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83:I83">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78:I79">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D85:I86">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D86:I88">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D94:G94">
     <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D67:G67">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D77:G77">
-    <cfRule type="colorScale" priority="34">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D78:G79">
-    <cfRule type="colorScale" priority="33">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D76:G76">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H77:I77">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D95:G96">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D93:G93">
     <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
@@ -3100,7 +3268,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H78:I79">
+  <conditionalFormatting sqref="D103:G103">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
@@ -3112,7 +3280,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H76:I76">
+  <conditionalFormatting sqref="D104:G105">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="min"/>
@@ -3124,7 +3292,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D84:G84">
+  <conditionalFormatting sqref="D102:G102">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
@@ -3136,19 +3304,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D85:G86">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D83:G83">
+  <conditionalFormatting sqref="H103:I103">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
@@ -3160,7 +3316,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H84:I84">
+  <conditionalFormatting sqref="H104:I105">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -3172,7 +3328,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H85:I86">
+  <conditionalFormatting sqref="H102:I102">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -3184,7 +3340,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H83:I83">
+  <conditionalFormatting sqref="D110:G110">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -3196,43 +3352,43 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D78:I79">
+  <conditionalFormatting sqref="D111:G112">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D85:I86">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D109:G109">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D86:I88">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H110:I110">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D94:G94">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H111:I112">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -3244,7 +3400,55 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D95:G96">
+  <conditionalFormatting sqref="H109:I109">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D104:I105">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D111:I112">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D112:I112">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D96:G96">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -3256,163 +3460,115 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D93:G93">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D103:G103">
-    <cfRule type="colorScale" priority="16">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104:G105">
-    <cfRule type="colorScale" priority="15">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D102:G102">
-    <cfRule type="colorScale" priority="14">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H103:I103">
+  <conditionalFormatting sqref="D8:G8">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H104:I105">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9:G9">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H102:I102">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D17:G17">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D110:G110">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:G18">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D111:G112">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D36:G36">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D109:G109">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D37:G37">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H110:I110">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:G27">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H111:I112">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:G28">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H109:I109">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47:G47">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D104:I105">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48:G48">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -3424,7 +3580,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D111:I112">
+  <conditionalFormatting sqref="D56:G56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3436,7 +3592,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D112:I112">
+  <conditionalFormatting sqref="D57:G57">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>